<commit_message>
created function to copy sheet within same workbook
</commit_message>
<xml_diff>
--- a/tests/sample_data/test_workbook.xlsx
+++ b/tests/sample_data/test_workbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fosa/PythonProjects/git_tree/auditing_automation/xlwings_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/fosa/pythonprojects/git_tree/auditing_automation/tests/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71E5555-928C-2C42-A1B5-C841C50DAB7A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0862BD8D-E118-A347-95C4-B34FFC5035CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="13900" xr2:uid="{6D501CA2-B23A-2B48-B2C2-E8CE2BD33026}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>